<commit_message>
Promena specifikacije potenciometra, 06.06.2020.
</commit_message>
<xml_diff>
--- a/BOM_Signal_Generator_Verzija_SMD.xlsx
+++ b/BOM_Signal_Generator_Verzija_SMD.xlsx
@@ -216,9 +216,6 @@
     <t>75-MKP1839447161</t>
   </si>
   <si>
-    <t xml:space="preserve">858-P0925NFC15BR20K </t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -633,6 +630,9 @@
   </si>
   <si>
     <t>Total with VAT</t>
+  </si>
+  <si>
+    <t>652-3310H-001-203L</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1036,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1134,22 +1134,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1157,9 +1145,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1468,7 +1469,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,16 +1485,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="43"/>
+      <c r="A1" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1512,13 +1513,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1526,16 +1527,16 @@
         <v>37</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="7">
         <v>5.9</v>
@@ -1545,7 +1546,7 @@
         <v>5.9</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1553,16 +1554,16 @@
         <v>55</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="11">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" s="11">
         <v>6.17</v>
@@ -1572,24 +1573,24 @@
         <v>6.17</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="11">
         <v>8.17</v>
@@ -1599,15 +1600,15 @@
         <v>8.17</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>48</v>
@@ -1616,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F6" s="11">
         <v>1.43</v>
@@ -1629,7 +1630,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
@@ -1641,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="11">
         <v>0.52400000000000002</v>
@@ -1654,7 +1655,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>24</v>
@@ -1679,10 +1680,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>48</v>
@@ -1691,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" s="15">
         <v>1.2</v>
@@ -1704,19 +1705,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="D10" s="11">
-        <v>1</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>115</v>
       </c>
       <c r="F10" s="15">
         <v>3.46</v>
@@ -1729,7 +1730,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>23</v>
@@ -1754,10 +1755,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>50</v>
@@ -1766,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="11">
         <v>0.38</v>
@@ -1800,7 +1801,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>33</v>
@@ -1825,7 +1826,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>35</v>
@@ -1850,13 +1851,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="11">
         <v>2</v>
@@ -1899,7 +1900,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>57</v>
@@ -1908,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" s="11">
         <v>1.45</v>
@@ -1921,44 +1922,44 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="11">
         <v>1</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>65</v>
+      <c r="E19" s="53" t="s">
+        <v>199</v>
       </c>
       <c r="F19" s="11">
-        <v>2.71</v>
+        <v>6.72</v>
       </c>
       <c r="G19" s="12">
         <f t="shared" si="0"/>
-        <v>2.71</v>
+        <v>6.72</v>
       </c>
       <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="11">
         <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" s="11">
         <v>1.05</v>
@@ -1971,7 +1972,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B21" s="11">
         <v>200</v>
@@ -1996,7 +1997,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>16</v>
@@ -2008,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" s="11">
         <v>1.41</v>
@@ -2021,7 +2022,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" s="11">
         <v>500</v>
@@ -2033,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F23" s="11">
         <v>1.39</v>
@@ -2046,13 +2047,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="11">
         <v>2</v>
@@ -2069,13 +2070,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25" s="11">
         <v>100</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="11">
         <v>3</v>
@@ -2092,13 +2093,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" s="11">
         <v>100</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="11">
         <v>1</v>
@@ -2110,18 +2111,18 @@
         <v>0</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="11">
         <v>2</v>
@@ -2133,18 +2134,18 @@
         <v>0</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="11">
         <v>2</v>
@@ -2161,13 +2162,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="11">
         <v>1</v>
@@ -2179,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2190,7 +2191,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="11">
         <v>1</v>
@@ -2202,18 +2203,18 @@
         <v>0</v>
       </c>
       <c r="H30" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="11">
         <v>1</v>
@@ -2225,18 +2226,18 @@
         <v>0</v>
       </c>
       <c r="H31" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B32" s="11">
         <v>510</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="11">
         <v>5</v>
@@ -2248,18 +2249,18 @@
         <v>0</v>
       </c>
       <c r="H32" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" s="11">
         <v>510</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="11">
         <v>2</v>
@@ -2276,13 +2277,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="11">
         <v>4</v>
@@ -2294,18 +2295,18 @@
         <v>0</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="11">
         <v>1</v>
@@ -2317,18 +2318,18 @@
         <v>0</v>
       </c>
       <c r="H35" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="11">
         <v>2</v>
@@ -2340,18 +2341,18 @@
         <v>0</v>
       </c>
       <c r="H36" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D37" s="11">
         <v>2</v>
@@ -2363,18 +2364,18 @@
         <v>0</v>
       </c>
       <c r="H37" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38" s="11">
         <v>1</v>
@@ -2386,18 +2387,18 @@
         <v>0</v>
       </c>
       <c r="H38" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="11">
         <v>1</v>
@@ -2409,18 +2410,18 @@
         <v>0</v>
       </c>
       <c r="H39" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="11">
         <v>1</v>
@@ -2432,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2440,10 +2441,10 @@
         <v>31</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" s="11">
         <v>1</v>
@@ -2455,18 +2456,18 @@
         <v>0</v>
       </c>
       <c r="H41" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="11">
         <v>1</v>
@@ -2478,18 +2479,18 @@
         <v>0</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D43" s="11">
         <v>2</v>
@@ -2501,18 +2502,18 @@
         <v>0</v>
       </c>
       <c r="H43" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" s="11">
         <v>1</v>
@@ -2524,18 +2525,18 @@
         <v>0</v>
       </c>
       <c r="H44" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D45" s="11">
         <v>1</v>
@@ -2547,18 +2548,18 @@
         <v>0</v>
       </c>
       <c r="H45" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D46" s="11">
         <v>1</v>
@@ -2570,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2578,10 +2579,10 @@
         <v>36</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D47" s="11">
         <v>1</v>
@@ -2593,18 +2594,18 @@
         <v>0</v>
       </c>
       <c r="H47" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="11">
         <v>4</v>
@@ -2616,18 +2617,18 @@
         <v>0</v>
       </c>
       <c r="H48" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B49" s="11">
         <v>62</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49" s="11">
         <v>1</v>
@@ -2639,18 +2640,18 @@
         <v>0</v>
       </c>
       <c r="H49" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B50" s="11">
         <v>56</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D50" s="11">
         <v>1</v>
@@ -2662,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2723,13 +2724,13 @@
         <v>6</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D53" s="11">
         <v>2</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F53" s="11">
         <v>1.21</v>
@@ -2739,7 +2740,7 @@
         <v>2.42</v>
       </c>
       <c r="H53" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2750,13 +2751,13 @@
         <v>7</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D54" s="11">
         <v>2</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F54" s="11">
         <v>0.14000000000000001</v>
@@ -2766,12 +2767,12 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H54" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>18</v>
@@ -2789,12 +2790,12 @@
         <v>0</v>
       </c>
       <c r="H55" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>27</v>
@@ -2812,24 +2813,24 @@
         <v>0</v>
       </c>
       <c r="H56" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B57" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>127</v>
-      </c>
       <c r="D57" s="11">
         <v>1</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F57" s="11">
         <v>0.52</v>
@@ -2839,24 +2840,24 @@
         <v>0.52</v>
       </c>
       <c r="H57" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" s="11">
+        <v>1</v>
+      </c>
+      <c r="E58" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="D58" s="11">
-        <v>1</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>128</v>
       </c>
       <c r="F58" s="11">
         <v>1.23</v>
@@ -2866,12 +2867,12 @@
         <v>1.23</v>
       </c>
       <c r="H58" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>62</v>
@@ -2889,12 +2890,12 @@
         <v>0</v>
       </c>
       <c r="H59" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>4</v>
@@ -2906,7 +2907,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" s="11">
         <v>0.27100000000000002</v>
@@ -2919,19 +2920,19 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="D61" s="11">
         <v>2</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F61" s="11">
         <v>0.60299999999999998</v>
@@ -2946,13 +2947,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B62" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="D62" s="11">
         <v>1</v>
@@ -2964,24 +2965,24 @@
         <v>0</v>
       </c>
       <c r="H62" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D63" s="23">
         <v>11</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F63" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2991,24 +2992,24 @@
         <v>0.77</v>
       </c>
       <c r="H63" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D64" s="11">
         <v>1</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F64" s="11">
         <v>0.3</v>
@@ -3023,19 +3024,19 @@
     </row>
     <row r="65" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D65" s="26">
         <v>10</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F65" s="26">
         <v>0.28000000000000003</v>
@@ -3045,18 +3046,18 @@
         <v>2.8000000000000003</v>
       </c>
       <c r="H65" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D66" s="26">
         <v>2</v>
@@ -3065,18 +3066,18 @@
       <c r="F66" s="26"/>
       <c r="G66" s="27"/>
       <c r="H66" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D67" s="26">
         <v>1</v>
@@ -3085,18 +3086,18 @@
       <c r="F67" s="26"/>
       <c r="G67" s="27"/>
       <c r="H67" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D68" s="29">
         <v>1</v>
@@ -3108,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3118,32 +3119,32 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52"/>
       <c r="F69" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G69" s="34">
         <f>SUM(G3:G68)</f>
-        <v>67.344999999999999</v>
+        <v>71.35499999999999</v>
       </c>
       <c r="H69" s="35"/>
     </row>
     <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="44"/>
-      <c r="B70" s="45"/>
-      <c r="C70" s="46" t="s">
+      <c r="A70" s="41"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" s="49"/>
+      <c r="E70" s="45">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F70" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="D70" s="46"/>
-      <c r="E70" s="49">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="F70" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="G70" s="48">
+      <c r="G70" s="44">
         <f>G69*(1+E70)</f>
-        <v>72.530564999999996</v>
-      </c>
-      <c r="H70" s="44"/>
+        <v>76.849334999999982</v>
+      </c>
+      <c r="H70" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>